<commit_message>
Reference to rev 1.1
</commit_message>
<xml_diff>
--- a/hw/BeeGl_Broker_Variant_B_BOM_rev1.0.xlsx
+++ b/hw/BeeGl_Broker_Variant_B_BOM_rev1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="360" windowWidth="28515" windowHeight="12315" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="360" windowWidth="28515" windowHeight="12315" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="2" r:id="rId1"/>
@@ -16,7 +16,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Load Cells Frame'!$A$1:$G$16</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -128,9 +127,6 @@
     <t>Component came</t>
   </si>
   <si>
-    <t>BeeGl_Broker_VariantB_Drawings_rev_1.0.pdf</t>
-  </si>
-  <si>
     <t>Straight Bar Load Cell Bottom Edge</t>
   </si>
   <si>
@@ -392,6 +388,9 @@
   </si>
   <si>
     <t>M5x10 Hexagon socket Head Cap Screw</t>
+  </si>
+  <si>
+    <t>BeeGl_Broker_VariantB_Drawings_rev_1.1.pdf</t>
   </si>
 </sst>
 </file>
@@ -1261,56 +1260,56 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="39.75" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45">
       <c r="A4" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30">
       <c r="B7" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="B8" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1318,7 +1317,7 @@
         <v>43705</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1359,7 +1358,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>31</v>
@@ -1382,7 +1381,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>21</v>
@@ -1402,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>25</v>
@@ -1422,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>23</v>
@@ -1442,7 +1441,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>24</v>
@@ -1462,7 +1461,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>27</v>
@@ -1482,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1499,7 +1498,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>29</v>
@@ -1510,16 +1509,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -1528,17 +1527,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -1547,17 +1546,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -1566,17 +1565,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12">
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30">
@@ -1584,16 +1583,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13">
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1601,13 +1600,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45">
@@ -1615,17 +1614,17 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -1634,17 +1633,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -1653,17 +1652,17 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17">
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -1672,13 +1671,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45">
@@ -1686,20 +1685,20 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="45">
@@ -1707,20 +1706,20 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="45">
@@ -1728,20 +1727,20 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45">
@@ -1749,20 +1748,20 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="45">
@@ -1770,20 +1769,20 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="135">
@@ -1791,17 +1790,17 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -1810,17 +1809,17 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -1843,7 +1842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -1871,7 +1870,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>31</v>
@@ -1894,7 +1893,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>21</v>
@@ -1914,7 +1913,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>25</v>
@@ -1934,7 +1933,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>23</v>
@@ -1954,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>24</v>
@@ -1974,7 +1973,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>27</v>
@@ -1994,7 +1993,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2011,7 +2010,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>29</v>
@@ -2022,16 +2021,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -2040,17 +2039,17 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -2059,17 +2058,17 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -2078,17 +2077,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12">
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30">
@@ -2096,16 +2095,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13">
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2113,13 +2112,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45">
@@ -2127,17 +2126,17 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15">
         <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -2146,17 +2145,17 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16">
         <v>2</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -2165,17 +2164,17 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17">
         <v>4</v>
       </c>
       <c r="E17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -2184,13 +2183,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="45">
@@ -2198,20 +2197,20 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30">
@@ -2219,20 +2218,20 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30">
@@ -2240,20 +2239,20 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45">
@@ -2261,20 +2260,20 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="45">
@@ -2282,20 +2281,20 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="45">
@@ -2312,7 +2311,7 @@
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>30</v>
@@ -2323,16 +2322,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45">
@@ -2340,16 +2339,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="30">
@@ -2357,16 +2356,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="135">
@@ -2374,17 +2373,17 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -2393,17 +2392,17 @@
         <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -2429,8 +2428,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9:F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2456,7 +2455,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>31</v>
@@ -2470,16 +2469,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2487,16 +2486,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2504,16 +2503,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45">
@@ -2521,19 +2520,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" hidden="1">
@@ -2541,19 +2540,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6">
         <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30" hidden="1">
@@ -2561,19 +2560,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" hidden="1">
@@ -2581,19 +2580,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8">
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45">
@@ -2601,16 +2600,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45">
@@ -2618,16 +2617,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="45">
@@ -2635,16 +2634,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11">
         <v>10</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30">
@@ -2652,16 +2651,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12">
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30">
@@ -2669,16 +2668,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D13">
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" hidden="1">
@@ -2686,19 +2685,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>101</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" hidden="1">
@@ -2715,7 +2714,7 @@
         <v>4</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>26</v>
@@ -2726,16 +2725,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16">
         <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>